<commit_message>
Final report and Best practices
</commit_message>
<xml_diff>
--- a/Data/Input/Entry_ProductList.xlsx
+++ b/Data/Input/Entry_ProductList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/160dd9a03bb2187c/Documents/UiPath/Dermalogica_InternetPriceMonitoring/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{FFBF7E02-C39D-4D7C-9613-679E190932D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A13C25E6-AD0F-4967-B69D-AC4621A5D1B0}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{FFBF7E02-C39D-4D7C-9613-679E190932D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC143AFC-7D0A-4FA3-A192-915A65B98FC8}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{207DB72F-33DF-4AF6-93DE-4A1FC0A8541C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>ml</t>
   </si>
@@ -257,24 +257,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri-Bold"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -386,6 +368,24 @@
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri-Bold"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -404,26 +404,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D838A936-9575-4DC1-8A1A-6982412EF0B2}" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D2" xr:uid="{D838A936-9575-4DC1-8A1A-6982412EF0B2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D838A936-9575-4DC1-8A1A-6982412EF0B2}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="0">
+  <autoFilter ref="A1:D11" xr:uid="{D838A936-9575-4DC1-8A1A-6982412EF0B2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{97A34F97-D1DB-4CCA-A87E-145F70C77184}" name="SKU" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{A4D29227-E006-4AF9-AC16-9EAFD98E9A37}" name="Item" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{FD94CD88-504E-4C8B-9B14-24B1F0BFB8EE}" name="Oz" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{8C5B7C45-EDCF-49C1-9108-F6EAC3A6709D}" name="ml" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{97A34F97-D1DB-4CCA-A87E-145F70C77184}" name="SKU" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A4D29227-E006-4AF9-AC16-9EAFD98E9A37}" name="Item" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{FD94CD88-504E-4C8B-9B14-24B1F0BFB8EE}" name="Oz" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{8C5B7C45-EDCF-49C1-9108-F6EAC3A6709D}" name="ml" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{37B2FFD0-81ED-4BC4-A86B-BF4F2386E1B0}" name="Table13" displayName="Table13" ref="A1:D22" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{37B2FFD0-81ED-4BC4-A86B-BF4F2386E1B0}" name="Table13" displayName="Table13" ref="A1:D22" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:D22" xr:uid="{D838A936-9575-4DC1-8A1A-6982412EF0B2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C74306C3-C5FA-4872-B34A-329FF3B41984}" name="SKU" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{A0EA9FFD-31DC-4376-91F6-C16120FDD2E4}" name="Item" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{9FDD85E7-76F7-4192-A498-494965A4B445}" name="Oz" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{E88187C5-8A8D-4624-B6C5-CB39A8AF349C}" name="ml" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C74306C3-C5FA-4872-B34A-329FF3B41984}" name="SKU" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{A0EA9FFD-31DC-4376-91F6-C16120FDD2E4}" name="Item" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9FDD85E7-76F7-4192-A498-494965A4B445}" name="Oz" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{E88187C5-8A8D-4624-B6C5-CB39A8AF349C}" name="ml" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -746,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49ACA679-30E4-4595-A820-6C8DC4737B98}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -785,6 +785,132 @@
       </c>
       <c r="D2" s="1">
         <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>111266</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>101106</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>101104</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>110616</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>111249</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>111252</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>111059</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>111064</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="D10" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>111060</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -800,7 +926,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>